<commit_message>
added enhanced versions controls to the always@ and changed/fixed some of the control signals sheet
</commit_message>
<xml_diff>
--- a/control signals.xlsx
+++ b/control signals.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>T1</t>
   </si>
@@ -90,13 +90,10 @@
     <t>Ryout, ADDRin</t>
   </si>
   <si>
-    <t>Rxout, DOUTin, W, Done?</t>
-  </si>
-  <si>
-    <t>G != 0 else Done</t>
-  </si>
-  <si>
-    <t>if(true)  Ryout, RXin, Done</t>
+    <t>G != 0 {Ryout, ADDRin} else Done</t>
+  </si>
+  <si>
+    <t>Rxout, DOUTin, W_D, Done?</t>
   </si>
 </sst>
 </file>
@@ -439,16 +436,16 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -574,7 +571,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -586,10 +583,10 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>

</xml_diff>

<commit_message>
added pin assignments and test.as script of program removed datain, dataout, address from mem.v slight changes to proc.v
</commit_message>
<xml_diff>
--- a/control signals.xlsx
+++ b/control signals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="7500" windowHeight="4860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>T1</t>
   </si>
@@ -94,6 +94,27 @@
   </si>
   <si>
     <t>Rxout, DOUTin, W_D, Done?</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>110</t>
   </si>
 </sst>
 </file>
@@ -436,7 +457,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,8 +466,7 @@
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -488,7 +508,9 @@
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -501,22 +523,25 @@
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>18</v>
@@ -533,7 +558,9 @@
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
         <v>18</v>
@@ -550,37 +577,41 @@
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
         <v>24</v>

</xml_diff>